<commit_message>
worked on covid and kpi dashboard
</commit_message>
<xml_diff>
--- a/dashboards/kpi dashboard.xlsx
+++ b/dashboards/kpi dashboard.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMING\PYTHON\PROJECTS\ds_projects\dashboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE78C0-F0B2-4F04-BBA2-B16B97E59B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -21,17 +22,23 @@
     <definedName name="cur_month">Dashboard!$F$6</definedName>
     <definedName name="cur_year">Dashboard!$F$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="95">
   <si>
     <t>Actual</t>
   </si>
@@ -290,12 +297,39 @@
   <si>
     <t/>
   </si>
+  <si>
+    <t>Calculations for scrolling table</t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Variance Actual to PY</t>
+  </si>
+  <si>
+    <t>Variance Actual to Budget</t>
+  </si>
+  <si>
+    <t>Revenue%</t>
+  </si>
+  <si>
+    <t>Profit%</t>
+  </si>
+  <si>
+    <t>Cash%</t>
+  </si>
+  <si>
+    <t>Unique Key</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,8 +352,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +421,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -447,11 +494,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -513,16 +632,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF77BBE2"/>
       <color rgb="FFCCE6F4"/>
-      <color rgb="FF77BBE2"/>
       <color rgb="FF638EC6"/>
     </mruColors>
   </colors>
@@ -538,7 +671,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="16" fmlaLink="Calculation!$D$4" fmlaRange="Calculation!$C$15:$C$17" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="16" fmlaLink="Calculation!$D$4" fmlaRange="Calculation!$C$15:$C$17" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,6 +697,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -621,7 +757,7 @@
         <xdr:cNvPr id="2" name="Flowchart: Process 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3011E72-2444-4441-961B-3CDE12AC0A6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -707,7 +843,7 @@
         <xdr:cNvPr id="3" name="Flowchart: Process 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{370A9D48-FA05-4A66-842B-7340C8262322}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -781,7 +917,7 @@
         <xdr:cNvPr id="4" name="Flowchart: Process 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{172F4739-0F78-4296-8129-EEAE0BEE939D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -855,7 +991,7 @@
         <xdr:cNvPr id="5" name="Flowchart: Process 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4D0F75-B6E2-4DAB-BA9D-74B16B7DCAD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -929,7 +1065,7 @@
         <xdr:cNvPr id="6" name="Flowchart: Process 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{379ABDD2-4D35-4D0F-B37D-7399B23E4C40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1015,7 +1151,7 @@
         <xdr:cNvPr id="7" name="Flowchart: Process 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57255CB9-D220-41C3-85B2-657B0CFE9BC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1101,7 +1237,7 @@
         <xdr:cNvPr id="8" name="Flowchart: Process 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0BE1059-7DD4-47D3-AAAA-CB2AFC43ED9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1187,7 +1323,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FF9A5DD-846E-4BF8-B1C1-72ECD93ED4BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1231,7 +1367,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B5B4492-B12B-4A46-BA4E-44911F8FFF2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1269,7 +1405,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525E2D28-78A3-410A-93BE-0F1987D2C417}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1327,7 +1463,7 @@
         <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5C48553-9E71-4B48-AF1B-4FBAED8198B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1385,7 +1521,7 @@
         <xdr:cNvPr id="13" name="TextBox 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{495C6891-8C5B-4E9F-8731-945CC1EFF1EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1448,7 +1584,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAA81D4-F84F-4A29-8061-FB4E50574823}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1745,11 +1881,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1906,7 @@
         <v>79</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.25">
@@ -1780,7 +1916,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Year Incorrect" error="Please input year as YYYY (4 digits). Thanks." promptTitle="Year" prompt="Please input year as YYYY" sqref="F5">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Year Incorrect" error="Please input year as YYYY (4 digits). Thanks." promptTitle="Year" prompt="Please input year as YYYY" sqref="F5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>4</formula1>
     </dataValidation>
   </dataValidations>
@@ -1818,7 +1954,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Month" prompt="Please select a month from the drop-down">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Month" prompt="Please select a month from the drop-down" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Calculation!$B$15:$B$26</xm:f>
           </x14:formula1>
@@ -1831,11 +1967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:AZ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C17"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35:AC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,26 +1980,215 @@
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B2" s="36" t="s">
         <v>82</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
+      <c r="M2" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>81</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="O8" t="str">
+        <f>O9&amp;O10&amp;O11&amp;O12</f>
+        <v>2017JunActualRevenue</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ref="P8:W8" si="0">P9&amp;P10&amp;P11&amp;P12</f>
+        <v>2017JunActualProfit</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunActualCash</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualRevenue</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualProfit</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualCash</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetRevenue</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetProfit</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetCash</v>
+      </c>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+      <c r="P9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+      <c r="Q9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+      <c r="R9">
+        <f>cur_year-1</f>
+        <v>2016</v>
+      </c>
+      <c r="S9">
+        <f>cur_year-1</f>
+        <v>2016</v>
+      </c>
+      <c r="T9">
+        <f>cur_year-1</f>
+        <v>2016</v>
+      </c>
+      <c r="U9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+      <c r="V9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+      <c r="W9">
+        <f>cur_year</f>
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="O10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="P10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="Q10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="R10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="S10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="T10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="U10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="V10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+      <c r="W10" t="str">
+        <f>cur_month</f>
+        <v>Jun</v>
+      </c>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="O12" t="str">
+        <f>O14</f>
+        <v>Revenue</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ref="P12:W12" si="1">P14</f>
+        <v>Profit</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="1"/>
+        <v>Cash</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="1"/>
+        <v>Revenue</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="1"/>
+        <v>Profit</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="1"/>
+        <v>Cash</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="1"/>
+        <v>Revenue</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="1"/>
+        <v>Profit</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="1"/>
+        <v>Cash</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
         <v>83</v>
       </c>
@@ -1875,20 +2200,96 @@
       </c>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
+      <c r="O13" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB13" s="45"/>
+      <c r="AC13" s="45"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="34" t="str">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G14" s="37" t="str">
         <f t="array" ref="G14:I14">TRANSPOSE(C15:C17)</f>
         <v>Productivity Apps</v>
       </c>
-      <c r="H14" s="34" t="str">
+      <c r="H14" s="38" t="str">
         <v>Game Apps</v>
       </c>
-      <c r="I14" s="34" t="str">
+      <c r="I14" s="39" t="str">
         <v>Utility Apps</v>
       </c>
+      <c r="M14" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1898,17 +2299,85 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="41" t="s">
         <v>65</v>
       </c>
+      <c r="M15">
+        <f>IF(N15&lt;&gt;"",ROW(A1),"")</f>
+        <v>1</v>
+      </c>
+      <c r="N15" t="str">
+        <f>IF(INDEX(G15:I15,1,$D$4)="","",INDEX(G15:I15,1,$D$4))</f>
+        <v>Fightrr</v>
+      </c>
+      <c r="O15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>11649</v>
+      </c>
+      <c r="P15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>802</v>
+      </c>
+      <c r="Q15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5956</v>
+      </c>
+      <c r="R15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>10414</v>
+      </c>
+      <c r="S15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>536</v>
+      </c>
+      <c r="T15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6713</v>
+      </c>
+      <c r="U15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>10593</v>
+      </c>
+      <c r="V15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>554</v>
+      </c>
+      <c r="W15">
+        <f>IF($N15&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N15,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6803</v>
+      </c>
+      <c r="X15" s="46">
+        <f>IFERROR((O15-R15)/R15,"")</f>
+        <v>0.11859035913193777</v>
+      </c>
+      <c r="Y15" s="46">
+        <f>IFERROR((P15-S15)/S15,"")</f>
+        <v>0.4962686567164179</v>
+      </c>
+      <c r="Z15" s="46">
+        <f>IFERROR((Q15-T15)/T15,"")</f>
+        <v>-0.11276627439296887</v>
+      </c>
+      <c r="AA15" s="47">
+        <f>IFERROR((O15-U15)/U15,"")</f>
+        <v>9.9688473520249218E-2</v>
+      </c>
+      <c r="AB15" s="47">
+        <f t="shared" ref="AB15:AC15" si="2">IFERROR((P15-V15)/V15,"")</f>
+        <v>0.44765342960288806</v>
+      </c>
+      <c r="AC15" s="47">
+        <f t="shared" si="2"/>
+        <v>-0.12450389534029105</v>
+      </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -1918,17 +2387,85 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="41" t="s">
         <v>66</v>
       </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M33" si="3">IF(N16&lt;&gt;"",ROW(A2),"")</f>
+        <v>2</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" ref="N16:N34" si="4">IF(INDEX(G16:I16,1,$D$4)="","",INDEX(G16:I16,1,$D$4))</f>
+        <v>Kryptis</v>
+      </c>
+      <c r="O16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7718</v>
+      </c>
+      <c r="P16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>876</v>
+      </c>
+      <c r="Q16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8432</v>
+      </c>
+      <c r="R16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7282</v>
+      </c>
+      <c r="S16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>775</v>
+      </c>
+      <c r="T16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8242</v>
+      </c>
+      <c r="U16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6409</v>
+      </c>
+      <c r="V16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>654</v>
+      </c>
+      <c r="W16">
+        <f>IF($N16&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N16,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8312</v>
+      </c>
+      <c r="X16" s="46">
+        <f t="shared" ref="X16:X34" si="5">IFERROR((O16-R16)/R16,"")</f>
+        <v>5.9873661082120298E-2</v>
+      </c>
+      <c r="Y16" s="46">
+        <f t="shared" ref="Y16:Y34" si="6">IFERROR((P16-S16)/S16,"")</f>
+        <v>0.13032258064516128</v>
+      </c>
+      <c r="Z16" s="46">
+        <f t="shared" ref="Z16:Z34" si="7">IFERROR((Q16-T16)/T16,"")</f>
+        <v>2.3052657122057753E-2</v>
+      </c>
+      <c r="AA16" s="47">
+        <f t="shared" ref="AA16:AA34" si="8">IFERROR((O16-U16)/U16,"")</f>
+        <v>0.20424403183023873</v>
+      </c>
+      <c r="AB16" s="47">
+        <f t="shared" ref="AB16:AB34" si="9">IFERROR((P16-V16)/V16,"")</f>
+        <v>0.33944954128440369</v>
+      </c>
+      <c r="AC16" s="47">
+        <f t="shared" ref="AC16:AC34" si="10">IFERROR((Q16-W16)/W16,"")</f>
+        <v>1.4436958614051972E-2</v>
+      </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1938,173 +2475,1528 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="41" t="s">
         <v>67</v>
       </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="4"/>
+        <v>Perino</v>
+      </c>
+      <c r="O17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>15033</v>
+      </c>
+      <c r="P17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>469</v>
+      </c>
+      <c r="Q17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>3512</v>
+      </c>
+      <c r="R17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>15064</v>
+      </c>
+      <c r="S17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>392</v>
+      </c>
+      <c r="T17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>3488</v>
+      </c>
+      <c r="U17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>12724</v>
+      </c>
+      <c r="V17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>530</v>
+      </c>
+      <c r="W17">
+        <f>IF($N17&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N17,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>3347</v>
+      </c>
+      <c r="X17" s="46">
+        <f t="shared" si="5"/>
+        <v>-2.0578863515666491E-3</v>
+      </c>
+      <c r="Y17" s="46">
+        <f t="shared" si="6"/>
+        <v>0.19642857142857142</v>
+      </c>
+      <c r="Z17" s="46">
+        <f t="shared" si="7"/>
+        <v>6.8807339449541288E-3</v>
+      </c>
+      <c r="AA17" s="47">
+        <f t="shared" si="8"/>
+        <v>0.18146809179503301</v>
+      </c>
+      <c r="AB17" s="47">
+        <f t="shared" si="9"/>
+        <v>-0.11509433962264151</v>
+      </c>
+      <c r="AC17" s="47">
+        <f t="shared" si="10"/>
+        <v>4.9297878697340904E-2</v>
+      </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="41" t="s">
         <v>68</v>
       </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="4"/>
+        <v>Five Labs</v>
+      </c>
+      <c r="O18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>21579</v>
+      </c>
+      <c r="P18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>920</v>
+      </c>
+      <c r="Q18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7461</v>
+      </c>
+      <c r="R18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>20686</v>
+      </c>
+      <c r="S18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>653</v>
+      </c>
+      <c r="T18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8589</v>
+      </c>
+      <c r="U18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>20478</v>
+      </c>
+      <c r="V18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>658</v>
+      </c>
+      <c r="W18">
+        <f>IF($N18&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N18,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7602</v>
+      </c>
+      <c r="X18" s="46">
+        <f t="shared" si="5"/>
+        <v>4.3169293241806052E-2</v>
+      </c>
+      <c r="Y18" s="46">
+        <f t="shared" si="6"/>
+        <v>0.40888208269525267</v>
+      </c>
+      <c r="Z18" s="46">
+        <f t="shared" si="7"/>
+        <v>-0.13133077191756898</v>
+      </c>
+      <c r="AA18" s="47">
+        <f t="shared" si="8"/>
+        <v>5.3765016114854965E-2</v>
+      </c>
+      <c r="AB18" s="47">
+        <f t="shared" si="9"/>
+        <v>0.3981762917933131</v>
+      </c>
+      <c r="AC18" s="47">
+        <f t="shared" si="10"/>
+        <v>-1.8547750591949488E-2</v>
+      </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="41" t="s">
         <v>69</v>
       </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="4"/>
+        <v>Twistrr</v>
+      </c>
+      <c r="O19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>27210.600000000002</v>
+      </c>
+      <c r="P19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2903.4</v>
+      </c>
+      <c r="Q19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>10490.4</v>
+      </c>
+      <c r="R19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>25448.400000000001</v>
+      </c>
+      <c r="S19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2160</v>
+      </c>
+      <c r="T19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>11181.6</v>
+      </c>
+      <c r="U19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>24219</v>
+      </c>
+      <c r="V19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2520</v>
+      </c>
+      <c r="W19">
+        <f>IF($N19&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N19,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>10458</v>
+      </c>
+      <c r="X19" s="46">
+        <f t="shared" si="5"/>
+        <v>6.9246003678030868E-2</v>
+      </c>
+      <c r="Y19" s="46">
+        <f t="shared" si="6"/>
+        <v>0.34416666666666673</v>
+      </c>
+      <c r="Z19" s="46">
+        <f t="shared" si="7"/>
+        <v>-6.1815840309079266E-2</v>
+      </c>
+      <c r="AA19" s="47">
+        <f t="shared" si="8"/>
+        <v>0.12352285395763665</v>
+      </c>
+      <c r="AB19" s="47">
+        <f t="shared" si="9"/>
+        <v>0.15214285714285719</v>
+      </c>
+      <c r="AC19" s="47">
+        <f t="shared" si="10"/>
+        <v>3.0981067125645089E-3</v>
+      </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="41" t="s">
         <v>70</v>
       </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="4"/>
+        <v>Hackrr</v>
+      </c>
+      <c r="O20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>18700.5</v>
+      </c>
+      <c r="P20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>984.90000000000009</v>
+      </c>
+      <c r="Q20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>12654.6</v>
+      </c>
+      <c r="R20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>18471.600000000002</v>
+      </c>
+      <c r="S20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>663.6</v>
+      </c>
+      <c r="T20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>13127.1</v>
+      </c>
+      <c r="U20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>19101.600000000002</v>
+      </c>
+      <c r="V20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1302</v>
+      </c>
+      <c r="W20">
+        <f>IF($N20&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N20,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>12188.4</v>
+      </c>
+      <c r="X20" s="46">
+        <f t="shared" si="5"/>
+        <v>1.2391996361982599E-2</v>
+      </c>
+      <c r="Y20" s="46">
+        <f t="shared" si="6"/>
+        <v>0.4841772151898735</v>
+      </c>
+      <c r="Z20" s="46">
+        <f t="shared" si="7"/>
+        <v>-3.5994240921452564E-2</v>
+      </c>
+      <c r="AA20" s="47">
+        <f t="shared" si="8"/>
+        <v>-2.0998240985048485E-2</v>
+      </c>
+      <c r="AB20" s="47">
+        <f t="shared" si="9"/>
+        <v>-0.24354838709677412</v>
+      </c>
+      <c r="AC20" s="47">
+        <f t="shared" si="10"/>
+        <v>3.8249483115093103E-2</v>
+      </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="41" t="s">
         <v>71</v>
       </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="4"/>
+        <v>Pes</v>
+      </c>
+      <c r="O21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>45315.9</v>
+      </c>
+      <c r="P21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1932</v>
+      </c>
+      <c r="Q21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>15668.1</v>
+      </c>
+      <c r="R21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>43440.6</v>
+      </c>
+      <c r="S21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1371.3</v>
+      </c>
+      <c r="T21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>18036.900000000001</v>
+      </c>
+      <c r="U21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>43003.8</v>
+      </c>
+      <c r="V21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1381.8</v>
+      </c>
+      <c r="W21">
+        <f>IF($N21&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N21,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>15964.2</v>
+      </c>
+      <c r="X21" s="46">
+        <f t="shared" si="5"/>
+        <v>4.3169293241806121E-2</v>
+      </c>
+      <c r="Y21" s="46">
+        <f t="shared" si="6"/>
+        <v>0.40888208269525272</v>
+      </c>
+      <c r="Z21" s="46">
+        <f t="shared" si="7"/>
+        <v>-0.13133077191756903</v>
+      </c>
+      <c r="AA21" s="47">
+        <f t="shared" si="8"/>
+        <v>5.376501611485493E-2</v>
+      </c>
+      <c r="AB21" s="47">
+        <f t="shared" si="9"/>
+        <v>0.3981762917933131</v>
+      </c>
+      <c r="AC21" s="47">
+        <f t="shared" si="10"/>
+        <v>-1.8547750591949509E-2</v>
+      </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="41" t="s">
         <v>72</v>
       </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="4"/>
+        <v>Baden</v>
+      </c>
+      <c r="O22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>35980</v>
+      </c>
+      <c r="P22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2332</v>
+      </c>
+      <c r="Q22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>14274</v>
+      </c>
+      <c r="R22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>32790</v>
+      </c>
+      <c r="S22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2006</v>
+      </c>
+      <c r="T22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>14846</v>
+      </c>
+      <c r="U22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>36362</v>
+      </c>
+      <c r="V22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>2446</v>
+      </c>
+      <c r="W22">
+        <f>IF($N22&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N22,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>16392</v>
+      </c>
+      <c r="X22" s="46">
+        <f t="shared" si="5"/>
+        <v>9.728575785300396E-2</v>
+      </c>
+      <c r="Y22" s="46">
+        <f t="shared" si="6"/>
+        <v>0.16251246261216351</v>
+      </c>
+      <c r="Z22" s="46">
+        <f t="shared" si="7"/>
+        <v>-3.8528896672504379E-2</v>
+      </c>
+      <c r="AA22" s="47">
+        <f t="shared" si="8"/>
+        <v>-1.0505472746273583E-2</v>
+      </c>
+      <c r="AB22" s="47">
+        <f t="shared" si="9"/>
+        <v>-4.6606704824202781E-2</v>
+      </c>
+      <c r="AC22" s="47">
+        <f t="shared" si="10"/>
+        <v>-0.12920937042459738</v>
+      </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="41" t="s">
         <v>73</v>
       </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="4"/>
+        <v>Jellyfish</v>
+      </c>
+      <c r="O23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7657</v>
+      </c>
+      <c r="P23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>276</v>
+      </c>
+      <c r="Q23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5353</v>
+      </c>
+      <c r="R23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5307</v>
+      </c>
+      <c r="S23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>170</v>
+      </c>
+      <c r="T23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>4710</v>
+      </c>
+      <c r="U23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6431</v>
+      </c>
+      <c r="V23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>179</v>
+      </c>
+      <c r="W23">
+        <f>IF($N23&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N23,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5191</v>
+      </c>
+      <c r="X23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.44281138119464858</v>
+      </c>
+      <c r="Y23" s="46">
+        <f t="shared" si="6"/>
+        <v>0.62352941176470589</v>
+      </c>
+      <c r="Z23" s="46">
+        <f t="shared" si="7"/>
+        <v>0.13651804670912951</v>
+      </c>
+      <c r="AA23" s="47">
+        <f t="shared" si="8"/>
+        <v>0.19063909189861608</v>
+      </c>
+      <c r="AB23" s="47">
+        <f t="shared" si="9"/>
+        <v>0.54189944134078216</v>
+      </c>
+      <c r="AC23" s="47">
+        <f t="shared" si="10"/>
+        <v>3.1207859757272201E-2</v>
+      </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="41" t="s">
         <v>74</v>
       </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="4"/>
+        <v>Aviatrr</v>
+      </c>
+      <c r="O24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8126</v>
+      </c>
+      <c r="P24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>321</v>
+      </c>
+      <c r="Q24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6153</v>
+      </c>
+      <c r="R24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>9111</v>
+      </c>
+      <c r="S24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>567</v>
+      </c>
+      <c r="T24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5959</v>
+      </c>
+      <c r="U24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>8642</v>
+      </c>
+      <c r="V24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>554</v>
+      </c>
+      <c r="W24">
+        <f>IF($N24&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N24,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>7382</v>
+      </c>
+      <c r="X24" s="46">
+        <f t="shared" si="5"/>
+        <v>-0.10811107452529908</v>
+      </c>
+      <c r="Y24" s="46">
+        <f t="shared" si="6"/>
+        <v>-0.43386243386243384</v>
+      </c>
+      <c r="Z24" s="46">
+        <f t="shared" si="7"/>
+        <v>3.2555797952676623E-2</v>
+      </c>
+      <c r="AA24" s="47">
+        <f t="shared" si="8"/>
+        <v>-5.9708400833140475E-2</v>
+      </c>
+      <c r="AB24" s="47">
+        <f t="shared" si="9"/>
+        <v>-0.42057761732851984</v>
+      </c>
+      <c r="AC24" s="47">
+        <f t="shared" si="10"/>
+        <v>-0.16648604714169601</v>
+      </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="41" t="s">
         <v>75</v>
       </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="4"/>
+        <v>deRamblr</v>
+      </c>
+      <c r="O25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5272</v>
+      </c>
+      <c r="P25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>316</v>
+      </c>
+      <c r="Q25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1207</v>
+      </c>
+      <c r="R25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>4934</v>
+      </c>
+      <c r="S25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>233</v>
+      </c>
+      <c r="T25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1485</v>
+      </c>
+      <c r="U25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>4789</v>
+      </c>
+      <c r="V25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>215</v>
+      </c>
+      <c r="W25">
+        <f>IF($N25&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N25,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>1936</v>
+      </c>
+      <c r="X25" s="46">
+        <f t="shared" si="5"/>
+        <v>6.8504256181597084E-2</v>
+      </c>
+      <c r="Y25" s="46">
+        <f t="shared" si="6"/>
+        <v>0.35622317596566522</v>
+      </c>
+      <c r="Z25" s="46">
+        <f t="shared" si="7"/>
+        <v>-0.18720538720538721</v>
+      </c>
+      <c r="AA25" s="47">
+        <f t="shared" si="8"/>
+        <v>0.10085612862810607</v>
+      </c>
+      <c r="AB25" s="47">
+        <f t="shared" si="9"/>
+        <v>0.4697674418604651</v>
+      </c>
+      <c r="AC25" s="47">
+        <f t="shared" si="10"/>
+        <v>-0.37654958677685951</v>
+      </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="41" t="s">
         <v>76</v>
       </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="4"/>
+        <v>Arcade</v>
+      </c>
+      <c r="O26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6375</v>
+      </c>
+      <c r="P26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>192</v>
+      </c>
+      <c r="Q26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>4741</v>
+      </c>
+      <c r="R26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>6945</v>
+      </c>
+      <c r="S26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>309</v>
+      </c>
+      <c r="T26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5006</v>
+      </c>
+      <c r="U26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>5774</v>
+      </c>
+      <c r="V26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>350</v>
+      </c>
+      <c r="W26">
+        <f>IF($N26&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N26,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>4447</v>
+      </c>
+      <c r="X26" s="46">
+        <f t="shared" si="5"/>
+        <v>-8.2073434125269976E-2</v>
+      </c>
+      <c r="Y26" s="46">
+        <f t="shared" si="6"/>
+        <v>-0.37864077669902912</v>
+      </c>
+      <c r="Z26" s="46">
+        <f t="shared" si="7"/>
+        <v>-5.2936476228525771E-2</v>
+      </c>
+      <c r="AA26" s="47">
+        <f t="shared" si="8"/>
+        <v>0.10408728784205057</v>
+      </c>
+      <c r="AB26" s="47">
+        <f t="shared" si="9"/>
+        <v>-0.4514285714285714</v>
+      </c>
+      <c r="AC26" s="47">
+        <f t="shared" si="10"/>
+        <v>6.6111985608275248E-2</v>
+      </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G27" t="s">
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G27" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="41" t="s">
         <v>77</v>
       </c>
+      <c r="M27" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W27" t="str">
+        <f>IF($N27&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N27,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X27" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y27" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z27" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA27" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB27" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC27" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G28" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="41" t="s">
         <v>85</v>
       </c>
+      <c r="M28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W28" t="str">
+        <f>IF($N28&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N28,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X28" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y28" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z28" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA28" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB28" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC28" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G29" t="s">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G29" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="41" t="s">
         <v>85</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W29" t="str">
+        <f>IF($N29&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N29,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X29" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y29" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z29" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA29" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB29" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC29" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G30" s="40"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="41"/>
+      <c r="M30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W30" t="str">
+        <f>IF($N30&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N30,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X30" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y30" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z30" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA30" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB30" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC30" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G31" s="40"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="41"/>
+      <c r="M31" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W31" t="str">
+        <f>IF($N31&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N31,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X31" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y31" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z31" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA31" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB31" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC31" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G32" s="40"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="41"/>
+      <c r="M32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W32" t="str">
+        <f>IF($N32&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N32,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X32" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y32" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z32" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA32" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB32" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC32" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="7:52" x14ac:dyDescent="0.25">
+      <c r="G33" s="40"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="41"/>
+      <c r="M33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W33" t="str">
+        <f>IF($N33&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N33,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X33" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y33" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z33" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA33" s="47" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB33" s="47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC33" s="47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="7:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="42"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="43"/>
+      <c r="M34" s="44" t="str">
+        <f>IF(N34&lt;&gt;"",ROW(A20),"")</f>
+        <v/>
+      </c>
+      <c r="N34" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="S34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="T34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="U34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="V34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="W34" s="44" t="str">
+        <f>IF($N34&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N34,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v/>
+      </c>
+      <c r="X34" s="48" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y34" s="48" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z34" s="48" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AA34" s="49" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB34" s="49" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC34" s="49" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AD34" s="44"/>
+      <c r="AE34" s="44"/>
+      <c r="AF34" s="44"/>
+      <c r="AG34" s="44"/>
+      <c r="AH34" s="44"/>
+      <c r="AI34" s="44"/>
+      <c r="AJ34" s="44"/>
+      <c r="AK34" s="44"/>
+      <c r="AL34" s="44"/>
+      <c r="AM34" s="44"/>
+      <c r="AN34" s="44"/>
+      <c r="AO34" s="44"/>
+      <c r="AP34" s="44"/>
+      <c r="AQ34" s="44"/>
+      <c r="AR34" s="44"/>
+      <c r="AS34" s="44"/>
+      <c r="AT34" s="44"/>
+      <c r="AU34" s="44"/>
+      <c r="AV34" s="44"/>
+      <c r="AW34" s="44"/>
+      <c r="AX34" s="44"/>
+      <c r="AY34" s="44"/>
+      <c r="AZ34" s="44"/>
+    </row>
+    <row r="35" spans="7:52" x14ac:dyDescent="0.25">
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+    </row>
+    <row r="36" spans="7:52" x14ac:dyDescent="0.25">
+      <c r="N36" t="str">
+        <f>INDEX(G14:I14,D4)</f>
+        <v>Game Apps</v>
+      </c>
+      <c r="O36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!O$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>210616</v>
+      </c>
+      <c r="P36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!P$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>12324.3</v>
+      </c>
+      <c r="Q36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!Q$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>95902.1</v>
+      </c>
+      <c r="R36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!R$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>199893.6</v>
+      </c>
+      <c r="S36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!S$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>9835.9000000000015</v>
+      </c>
+      <c r="T36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!T$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>101383.6</v>
+      </c>
+      <c r="U36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!U$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>198526.40000000002</v>
+      </c>
+      <c r="V36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!V$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>11343.8</v>
+      </c>
+      <c r="W36">
+        <f>IF($N36&lt;&gt;"",INDEX(Data!$B$9:$J$51,MATCH(Calculation!$N36,Data!$A$9:$A$51,0),MATCH(Calculation!W$8,Data!$B$4:$J$4,0)),"")</f>
+        <v>100022.6</v>
+      </c>
+      <c r="X36" s="46">
+        <f t="shared" ref="X36" si="11">IFERROR((O36-R36)/R36,"")</f>
+        <v>5.3640536765559244E-2</v>
+      </c>
+      <c r="Y36" s="46">
+        <f t="shared" ref="Y36" si="12">IFERROR((P36-S36)/S36,"")</f>
+        <v>0.25299159202513216</v>
+      </c>
+      <c r="Z36" s="46">
+        <f t="shared" ref="Z36" si="13">IFERROR((Q36-T36)/T36,"")</f>
+        <v>-5.4066929957113374E-2</v>
+      </c>
+      <c r="AA36" s="47">
+        <f t="shared" ref="AA36" si="14">IFERROR((O36-U36)/U36,"")</f>
+        <v>6.0896686788255744E-2</v>
+      </c>
+      <c r="AB36" s="47">
+        <f t="shared" ref="AB36" si="15">IFERROR((P36-V36)/V36,"")</f>
+        <v>8.6434880727798452E-2</v>
+      </c>
+      <c r="AC36" s="47">
+        <f t="shared" ref="AC36" si="16">IFERROR((Q36-W36)/W36,"")</f>
+        <v>-4.1195689774111047E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2114,14 +4006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,264 +4096,408 @@
       <c r="AT3" s="14"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="D4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="18"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-      <c r="AR4" s="16"/>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="16"/>
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:AT4" si="0">B5&amp;B6&amp;B7&amp;B8</f>
+        <v>2017JunActualRevenue</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunActualProfit</v>
+      </c>
+      <c r="D4" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunActualCash</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualRevenue</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualProfit</v>
+      </c>
+      <c r="G4" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualCash</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetRevenue</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetProfit</v>
+      </c>
+      <c r="J4" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetCash</v>
+      </c>
+      <c r="K4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JanActualProfit</v>
+      </c>
+      <c r="L4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017FebActualProfit</v>
+      </c>
+      <c r="M4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017MarActualProfit</v>
+      </c>
+      <c r="N4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017AprActualProfit</v>
+      </c>
+      <c r="O4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017MayActualProfit</v>
+      </c>
+      <c r="P4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunActualProfit</v>
+      </c>
+      <c r="Q4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JulActualProfit</v>
+      </c>
+      <c r="R4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017AugActualProfit</v>
+      </c>
+      <c r="S4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017SepActualProfit</v>
+      </c>
+      <c r="T4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017OctActualProfit</v>
+      </c>
+      <c r="U4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017NovActualProfit</v>
+      </c>
+      <c r="V4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017DecActualProfit</v>
+      </c>
+      <c r="W4" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JanActualProfit</v>
+      </c>
+      <c r="X4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016FebActualProfit</v>
+      </c>
+      <c r="Y4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016MarActualProfit</v>
+      </c>
+      <c r="Z4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016AprActualProfit</v>
+      </c>
+      <c r="AA4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016MayActualProfit</v>
+      </c>
+      <c r="AB4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JunActualProfit</v>
+      </c>
+      <c r="AC4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016JulActualProfit</v>
+      </c>
+      <c r="AD4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016AugActualProfit</v>
+      </c>
+      <c r="AE4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016SepActualProfit</v>
+      </c>
+      <c r="AF4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016OctActualProfit</v>
+      </c>
+      <c r="AG4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2016NovActualProfit</v>
+      </c>
+      <c r="AH4" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>2016DecActualProfit</v>
+      </c>
+      <c r="AI4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JanBudgetProfit</v>
+      </c>
+      <c r="AJ4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017FebBudgetProfit</v>
+      </c>
+      <c r="AK4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017MarBudgetProfit</v>
+      </c>
+      <c r="AL4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017AprBudgetProfit</v>
+      </c>
+      <c r="AM4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017MayBudgetProfit</v>
+      </c>
+      <c r="AN4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JunBudgetProfit</v>
+      </c>
+      <c r="AO4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017JulBudgetProfit</v>
+      </c>
+      <c r="AP4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017AugBudgetProfit</v>
+      </c>
+      <c r="AQ4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017SepBudgetProfit</v>
+      </c>
+      <c r="AR4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017OctBudgetProfit</v>
+      </c>
+      <c r="AS4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017NovBudgetProfit</v>
+      </c>
+      <c r="AT4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2017DecBudgetProfit</v>
+      </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B5" s="19">
-        <f t="shared" ref="B5:D5" si="0">$A$2</f>
+        <f t="shared" ref="B5:D5" si="1">$A$2</f>
         <v>2017</v>
       </c>
       <c r="C5" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2017</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2017</v>
       </c>
       <c r="E5" s="19">
-        <f t="shared" ref="E5:G5" si="1">$B$2</f>
+        <f t="shared" ref="E5:G5" si="2">$B$2</f>
         <v>2016</v>
       </c>
       <c r="F5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2016</v>
       </c>
       <c r="G5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2016</v>
       </c>
       <c r="H5" s="19">
-        <f t="shared" ref="H5:J5" si="2">$A$2</f>
+        <f t="shared" ref="H5:J5" si="3">$A$2</f>
         <v>2017</v>
       </c>
       <c r="I5" s="19">
-        <f t="shared" si="2"/>
-        <v>2017</v>
-      </c>
-      <c r="J5" s="20">
-        <f t="shared" si="2"/>
-        <v>2017</v>
-      </c>
-      <c r="K5" s="21">
-        <f t="shared" ref="K5:V5" si="3">$A$2</f>
-        <v>2017</v>
-      </c>
-      <c r="L5" s="21">
         <f t="shared" si="3"/>
         <v>2017</v>
       </c>
-      <c r="M5" s="21">
+      <c r="J5" s="20">
         <f t="shared" si="3"/>
         <v>2017</v>
       </c>
+      <c r="K5" s="21">
+        <f t="shared" ref="K5:V5" si="4">$A$2</f>
+        <v>2017</v>
+      </c>
+      <c r="L5" s="21">
+        <f t="shared" si="4"/>
+        <v>2017</v>
+      </c>
+      <c r="M5" s="21">
+        <f t="shared" si="4"/>
+        <v>2017</v>
+      </c>
       <c r="N5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="O5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="P5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="Q5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="R5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="S5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="T5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="U5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="V5" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="W5" s="22">
-        <f t="shared" ref="W5:AH5" si="4">$B$2</f>
+        <f t="shared" ref="W5:AH5" si="5">$B$2</f>
         <v>2016</v>
       </c>
       <c r="X5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="Y5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="Z5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AA5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AB5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AC5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AD5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AE5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AF5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AG5" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AH5" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AI5" s="21">
-        <f t="shared" ref="AI5:AT5" si="5">$A$2</f>
+        <f t="shared" ref="AI5:AT5" si="6">$A$2</f>
         <v>2017</v>
       </c>
       <c r="AJ5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AK5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AL5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AM5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AN5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AO5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AP5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AQ5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AR5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AS5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
       <c r="AT5" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2017</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="str">
-        <f t="shared" ref="B6:J6" si="6">cur_month</f>
-        <v>Aug</v>
+        <f t="shared" ref="B6:J6" si="7">cur_month</f>
+        <v>Jun</v>
       </c>
       <c r="C6" s="19" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="D6" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="E6" s="19" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="F6" s="19" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="G6" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="H6" s="19" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="I6" s="19" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="J6" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Aug</v>
+        <f t="shared" si="7"/>
+        <v>Jun</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>21</v>
@@ -8280,7 +10316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>